<commit_message>
cmip5 --> cmip6 mappings
</commit_message>
<xml_diff>
--- a/mappings/seaice-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/seaice-cmip5-to-cmip6-mappings.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-seaice/mappings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqj34274/PycharmProjects/cmip6-specializations-seaice/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="-60" yWindow="480" windowWidth="22860" windowHeight="14520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Sea Ice</t>
   </si>
@@ -147,6 +147,48 @@
   </si>
   <si>
     <t>cmip6.seaice.thermodynamics.snow_processes.snow_ice_formation_scheme</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.grid.discretisation.vertical.layering</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.grid.discretisation.horizontal.thermodynamics_time_step</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.grid.discretisation.horizontal.dynamics_time_step</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.grid.discretisation.horizontal.grid</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.grid.discretisation.horizontal.scheme</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.dynamics.redistribution</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.radiative_processes.surface_albedo</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.thermodynamics.melt_ponds.formulation</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.thermodynamics.energy.basal_heat_flux</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.dynamics.transport_in_thickness_space</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.thermodynamics.energy.heat_diffusion</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.thermodynamics.mass.new_ice_formation</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.thermodynamics.snow_processes.redistribution</t>
+  </si>
+  <si>
+    <t>cmip6.seaice.dynamics.horizontal_transport</t>
   </si>
 </sst>
 </file>
@@ -267,7 +309,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -298,6 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1458,7 +1501,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1512,7 +1555,9 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
@@ -1521,7 +1566,7 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
@@ -1530,7 +1575,9 @@
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
@@ -1548,7 +1595,9 @@
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
@@ -1589,7 +1638,9 @@
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
@@ -1598,7 +1649,9 @@
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
@@ -1607,7 +1660,9 @@
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16"/>
+      <c r="C16" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
@@ -1627,7 +1682,7 @@
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
@@ -1636,7 +1691,9 @@
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
@@ -1670,7 +1727,9 @@
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
@@ -1688,7 +1747,9 @@
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
@@ -1697,7 +1758,9 @@
       <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
@@ -1706,7 +1769,9 @@
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
@@ -1726,8 +1791,8 @@
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>39</v>
+      <c r="C29" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
@@ -1737,7 +1802,7 @@
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
@@ -1746,7 +1811,9 @@
       <c r="B31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
@@ -1755,7 +1822,9 @@
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
@@ -1764,7 +1833,9 @@
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>